<commit_message>
Add a new test unit
</commit_message>
<xml_diff>
--- a/tests/testdata/test_transition_annot/WideTableForm_Annotation_ISTD_not_in_ISTDAnnot.xlsx
+++ b/tests/testdata/test_transition_annot/WideTableForm_Annotation_ISTD_not_in_ISTDAnnot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSOrganiser\tests\testdata\test_transition_annot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F01EC5E-1F1C-46E1-81B9-D8CA21E936D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333CD2BC-402A-4412-BA16-6213F383D9E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16770" windowHeight="8775" xr2:uid="{99D2A2AC-8431-4E91-B3F6-6736E2B6E0B0}"/>
   </bookViews>
@@ -628,7 +628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4803233F-B712-4161-B593-AE755CB87014}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -665,7 +667,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +675,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>